<commit_message>
imagenes modificadas y soporte para animaciones
</commit_message>
<xml_diff>
--- a/Documentacion/PlaneacionProyectoCotizadorAutos.xlsx
+++ b/Documentacion/PlaneacionProyectoCotizadorAutos.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="288" yWindow="48" windowWidth="11460" windowHeight="5568"/>
+    <workbookView xWindow="288" yWindow="48" windowWidth="11460" windowHeight="5568" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="Iteración 1" sheetId="1" r:id="rId1"/>
@@ -14,13 +14,14 @@
     <sheet name="US004" sheetId="5" r:id="rId5"/>
     <sheet name="US005" sheetId="6" r:id="rId6"/>
     <sheet name="US006" sheetId="7" r:id="rId7"/>
+    <sheet name="US007" sheetId="8" r:id="rId8"/>
   </sheets>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="265" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="291" uniqueCount="114">
   <si>
     <t>ID</t>
   </si>
@@ -347,6 +348,21 @@
   </si>
   <si>
     <t>Se desarrollará el plano general de la aplicación con el uso de la herramienta "Mockup" así como la generación de la maqueta basica de las vistas</t>
+  </si>
+  <si>
+    <t>US007</t>
+  </si>
+  <si>
+    <t>Unit testing</t>
+  </si>
+  <si>
+    <t>TA022</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>Se desarrollará la tecnología necesaria para asegurar la integridad y correcta función del código desarrollado</t>
   </si>
 </sst>
 </file>
@@ -707,7 +723,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="top"/>
@@ -816,6 +832,18 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1114,10 +1142,10 @@
   <sheetPr>
     <tabColor rgb="FFFFFF00"/>
   </sheetPr>
-  <dimension ref="B1:J31"/>
+  <dimension ref="B1:J36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+    <sheetView topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C32" sqref="C32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -1525,11 +1553,11 @@
       </c>
       <c r="F17" s="4">
         <f t="shared" ref="F17:G17" si="4">SUM(F18:F22)</f>
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="G17" s="4">
         <f t="shared" si="4"/>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="H17" s="4">
         <v>5</v>
@@ -1556,10 +1584,10 @@
       </c>
       <c r="F18" s="4">
         <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="G18" s="4">
         <v>2</v>
-      </c>
-      <c r="G18" s="4">
-        <v>0</v>
       </c>
       <c r="H18" s="4"/>
       <c r="I18" s="4" t="s">
@@ -1916,12 +1944,103 @@
         <v>64</v>
       </c>
       <c r="J31" s="4"/>
+    </row>
+    <row r="32" spans="2:10">
+      <c r="B32" s="6" t="s">
+        <v>109</v>
+      </c>
+      <c r="C32" s="7" t="s">
+        <v>110</v>
+      </c>
+      <c r="D32" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E32" s="4">
+        <f>SUM(E33:E36)</f>
+        <v>1</v>
+      </c>
+      <c r="F32" s="4">
+        <f t="shared" ref="F32:G32" si="7">SUM(F33:F36)</f>
+        <v>0</v>
+      </c>
+      <c r="G32" s="4">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="H32" s="4">
+        <v>6</v>
+      </c>
+      <c r="I32" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="J32" s="4" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="33" spans="2:10">
+      <c r="B33" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="C33" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="D33" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E33" s="39">
+        <v>1</v>
+      </c>
+      <c r="F33" s="39">
+        <f t="shared" ref="F33:F36" si="8">E33-G33</f>
+        <v>0</v>
+      </c>
+      <c r="G33" s="39" t="s">
+        <v>112</v>
+      </c>
+      <c r="H33" s="3"/>
+      <c r="I33" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="J33" s="3"/>
+    </row>
+    <row r="34" spans="2:10">
+      <c r="B34" s="37"/>
+      <c r="C34" s="38"/>
+      <c r="D34" s="38"/>
+      <c r="E34" s="38"/>
+      <c r="F34" s="38"/>
+      <c r="G34" s="38"/>
+      <c r="H34" s="38"/>
+      <c r="I34" s="38"/>
+      <c r="J34" s="38"/>
+    </row>
+    <row r="35" spans="2:10">
+      <c r="B35" s="37"/>
+      <c r="C35" s="38"/>
+      <c r="D35" s="38"/>
+      <c r="E35" s="38"/>
+      <c r="F35" s="38"/>
+      <c r="G35" s="38"/>
+      <c r="H35" s="38"/>
+      <c r="I35" s="38"/>
+      <c r="J35" s="38"/>
+    </row>
+    <row r="36" spans="2:10">
+      <c r="B36" s="37"/>
+      <c r="C36" s="38"/>
+      <c r="D36" s="38"/>
+      <c r="E36" s="38"/>
+      <c r="F36" s="38"/>
+      <c r="G36" s="38"/>
+      <c r="H36" s="38"/>
+      <c r="I36" s="38"/>
+      <c r="J36" s="38"/>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="B2:J2"/>
   </mergeCells>
-  <conditionalFormatting sqref="H23:H27 H9:H21 H29:H1048576 H1 H3:H7">
+  <conditionalFormatting sqref="H23:H27 H9:H21 H1 H3:H7 H29:H32 H34:H1048576">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="num" val="0"/>
@@ -2608,7 +2727,7 @@
   <dimension ref="B2:E11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+      <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -2737,4 +2856,130 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr>
+    <tabColor rgb="FF00B0F0"/>
+  </sheetPr>
+  <dimension ref="B2:E12"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4"/>
+  <cols>
+    <col min="1" max="1" width="2.88671875" style="2" customWidth="1"/>
+    <col min="2" max="2" width="17.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="40" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="52.88671875" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="16384" width="8.88671875" style="2"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:5" ht="30.6" customHeight="1" thickBot="1">
+      <c r="B2" s="30" t="s">
+        <v>83</v>
+      </c>
+      <c r="C2" s="30"/>
+      <c r="D2" s="30"/>
+      <c r="E2" s="30"/>
+    </row>
+    <row r="3" spans="2:5" ht="15" thickBot="1">
+      <c r="B3" s="18" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="24" t="s">
+        <v>109</v>
+      </c>
+      <c r="D3" s="25"/>
+      <c r="E3" s="26"/>
+    </row>
+    <row r="4" spans="2:5" ht="15" thickBot="1">
+      <c r="B4" s="18" t="s">
+        <v>76</v>
+      </c>
+      <c r="C4" s="24" t="s">
+        <v>110</v>
+      </c>
+      <c r="D4" s="25"/>
+      <c r="E4" s="26"/>
+    </row>
+    <row r="5" spans="2:5" ht="15" thickBot="1">
+      <c r="B5" s="18" t="s">
+        <v>79</v>
+      </c>
+      <c r="C5" s="24" t="s">
+        <v>111</v>
+      </c>
+      <c r="D5" s="25"/>
+      <c r="E5" s="26"/>
+    </row>
+    <row r="6" spans="2:5" ht="15" customHeight="1" thickBot="1">
+      <c r="B6" s="18" t="s">
+        <v>77</v>
+      </c>
+      <c r="C6" s="34" t="s">
+        <v>113</v>
+      </c>
+      <c r="D6" s="35"/>
+      <c r="E6" s="36"/>
+    </row>
+    <row r="7" spans="2:5" ht="15" thickBot="1">
+      <c r="B7" s="19" t="s">
+        <v>6</v>
+      </c>
+      <c r="C7" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="D7" s="11" t="s">
+        <v>76</v>
+      </c>
+      <c r="E7" s="12" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="8" spans="2:5" ht="15" thickBot="1">
+      <c r="C8" s="15" t="s">
+        <v>111</v>
+      </c>
+      <c r="D8" s="16" t="s">
+        <v>28</v>
+      </c>
+      <c r="E8" s="17" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="9" spans="2:5">
+      <c r="C9" s="37"/>
+      <c r="D9" s="38"/>
+      <c r="E9" s="40"/>
+    </row>
+    <row r="10" spans="2:5">
+      <c r="C10" s="37"/>
+      <c r="D10" s="38"/>
+      <c r="E10" s="40"/>
+    </row>
+    <row r="11" spans="2:5">
+      <c r="C11" s="37"/>
+      <c r="D11" s="38"/>
+      <c r="E11" s="40"/>
+    </row>
+    <row r="12" spans="2:5">
+      <c r="C12" s="38"/>
+      <c r="D12" s="38"/>
+      <c r="E12" s="38"/>
+    </row>
+  </sheetData>
+  <mergeCells count="5">
+    <mergeCell ref="B2:E2"/>
+    <mergeCell ref="C3:E3"/>
+    <mergeCell ref="C4:E4"/>
+    <mergeCell ref="C5:E5"/>
+    <mergeCell ref="C6:E6"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
nuevos formatos y cambio de periodo
</commit_message>
<xml_diff>
--- a/Documentacion/PlaneacionProyectoCotizadorAutos.xlsx
+++ b/Documentacion/PlaneacionProyectoCotizadorAutos.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="288" yWindow="48" windowWidth="11460" windowHeight="5568" activeTab="7"/>
+    <workbookView xWindow="288" yWindow="48" windowWidth="11460" windowHeight="5568"/>
   </bookViews>
   <sheets>
     <sheet name="Iteración 1" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="291" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="303" uniqueCount="124">
   <si>
     <t>ID</t>
   </si>
@@ -125,9 +125,6 @@
     <t xml:space="preserve">     Conexión a sitio</t>
   </si>
   <si>
-    <t>TA004,TA005,TA006,TA007,TA008</t>
-  </si>
-  <si>
     <t>US004</t>
   </si>
   <si>
@@ -363,13 +360,46 @@
   </si>
   <si>
     <t>Se desarrollará la tecnología necesaria para asegurar la integridad y correcta función del código desarrollado</t>
+  </si>
+  <si>
+    <t>TA023</t>
+  </si>
+  <si>
+    <t xml:space="preserve">     Compatibilidad con IE y Moz (Index DB)</t>
+  </si>
+  <si>
+    <t>TA004,TA005,TA006,TA007,TA008,TA023</t>
+  </si>
+  <si>
+    <t>TA024</t>
+  </si>
+  <si>
+    <t xml:space="preserve">     Validación de datos</t>
+  </si>
+  <si>
+    <t>TA015,TA016,TA017,TA024</t>
+  </si>
+  <si>
+    <t>Fernando, Nayeli</t>
+  </si>
+  <si>
+    <t xml:space="preserve">     Async tests</t>
+  </si>
+  <si>
+    <t xml:space="preserve">     Sync test</t>
+  </si>
+  <si>
+    <t>TA025</t>
+  </si>
+  <si>
+    <t>TA026</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="3">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -393,8 +423,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -419,6 +456,11 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="22">
     <border>
@@ -720,10 +762,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="top"/>
@@ -791,6 +834,18 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -833,20 +888,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="3" fillId="5" borderId="5" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="5" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Bad" xfId="1" builtinId="27"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1142,10 +1192,10 @@
   <sheetPr>
     <tabColor rgb="FFFFFF00"/>
   </sheetPr>
-  <dimension ref="B1:J36"/>
+  <dimension ref="B1:J38"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C32" sqref="C32"/>
+    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="87" zoomScaleNormal="87" workbookViewId="0">
+      <selection activeCell="J38" sqref="J38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -1165,17 +1215,17 @@
   <sheetData>
     <row r="1" spans="2:10" ht="6.6" customHeight="1"/>
     <row r="2" spans="2:10" ht="18">
-      <c r="B2" s="23" t="s">
-        <v>74</v>
-      </c>
-      <c r="C2" s="23"/>
-      <c r="D2" s="23"/>
-      <c r="E2" s="23"/>
-      <c r="F2" s="23"/>
-      <c r="G2" s="23"/>
-      <c r="H2" s="23"/>
-      <c r="I2" s="23"/>
-      <c r="J2" s="23"/>
+      <c r="B2" s="27" t="s">
+        <v>73</v>
+      </c>
+      <c r="C2" s="27"/>
+      <c r="D2" s="27"/>
+      <c r="E2" s="27"/>
+      <c r="F2" s="27"/>
+      <c r="G2" s="27"/>
+      <c r="H2" s="27"/>
+      <c r="I2" s="27"/>
+      <c r="J2" s="27"/>
     </row>
     <row r="3" spans="2:10" ht="7.2" customHeight="1"/>
     <row r="4" spans="2:10" ht="29.4" customHeight="1">
@@ -1192,7 +1242,7 @@
         <v>2</v>
       </c>
       <c r="F4" s="9" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="G4" s="9" t="s">
         <v>5</v>
@@ -1236,7 +1286,7 @@
         <v>16</v>
       </c>
       <c r="J5" s="5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="6" spans="2:10">
@@ -1253,7 +1303,7 @@
         <v>1</v>
       </c>
       <c r="F6" s="4">
-        <f t="shared" ref="F6:F31" si="1">E6-G6</f>
+        <f t="shared" ref="F6:F37" si="1">E6-G6</f>
         <v>0</v>
       </c>
       <c r="G6" s="4">
@@ -1270,7 +1320,7 @@
         <v>13</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D7" s="4" t="s">
         <v>11</v>
@@ -1293,10 +1343,10 @@
     </row>
     <row r="8" spans="2:10">
       <c r="B8" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="C8" s="4" t="s">
         <v>46</v>
-      </c>
-      <c r="C8" s="4" t="s">
-        <v>47</v>
       </c>
       <c r="D8" s="4" t="s">
         <v>11</v>
@@ -1380,7 +1430,7 @@
         <v>21</v>
       </c>
       <c r="C11" s="7" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D11" s="4" t="s">
         <v>8</v>
@@ -1390,12 +1440,12 @@
         <v>19</v>
       </c>
       <c r="F11" s="4">
-        <f t="shared" ref="F11:G11" si="3">SUM(F12:F16)</f>
-        <v>13</v>
+        <f t="shared" ref="F11:G11" si="3">SUM(F12:F17)</f>
+        <v>8</v>
       </c>
       <c r="G11" s="4">
         <f t="shared" si="3"/>
-        <v>6</v>
+        <v>29</v>
       </c>
       <c r="H11" s="4">
         <v>8</v>
@@ -1404,7 +1454,7 @@
         <v>16</v>
       </c>
       <c r="J11" s="5" t="s">
-        <v>34</v>
+        <v>115</v>
       </c>
     </row>
     <row r="12" spans="2:10">
@@ -1447,11 +1497,11 @@
         <v>5</v>
       </c>
       <c r="F13" s="4">
-        <f t="shared" si="1"/>
-        <v>1</v>
+        <f t="shared" ref="F13:F14" si="4">E13-G13</f>
+        <v>0</v>
       </c>
       <c r="G13" s="4">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="H13" s="4"/>
       <c r="I13" s="4" t="s">
@@ -1473,11 +1523,11 @@
         <v>5</v>
       </c>
       <c r="F14" s="4">
-        <f t="shared" si="1"/>
-        <v>4</v>
+        <f t="shared" si="4"/>
+        <v>0</v>
       </c>
       <c r="G14" s="4">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="H14" s="4"/>
       <c r="I14" s="4" t="s">
@@ -1499,11 +1549,11 @@
         <v>5</v>
       </c>
       <c r="F15" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" ref="C15:DY" si="5">E15-G15</f>
+        <v>0</v>
+      </c>
+      <c r="G15" s="4">
         <v>5</v>
-      </c>
-      <c r="G15" s="4">
-        <v>0</v>
       </c>
       <c r="H15" s="4"/>
       <c r="I15" s="4" t="s">
@@ -1512,267 +1562,267 @@
       <c r="J15" s="4"/>
     </row>
     <row r="16" spans="2:10">
-      <c r="B16" s="3" t="s">
+      <c r="B16" s="41" t="s">
         <v>32</v>
       </c>
-      <c r="C16" s="4" t="s">
+      <c r="C16" s="42" t="s">
         <v>33</v>
       </c>
-      <c r="D16" s="4" t="s">
+      <c r="D16" s="42" t="s">
         <v>11</v>
       </c>
-      <c r="E16" s="4">
+      <c r="E16" s="42">
         <v>3</v>
       </c>
-      <c r="F16" s="4">
+      <c r="F16" s="42">
+        <f>E16-G16</f>
+        <v>3</v>
+      </c>
+      <c r="G16" s="42">
+        <v>0</v>
+      </c>
+      <c r="H16" s="42"/>
+      <c r="I16" s="42" t="s">
+        <v>18</v>
+      </c>
+      <c r="J16" s="42"/>
+    </row>
+    <row r="17" spans="2:10">
+      <c r="B17" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>114</v>
+      </c>
+      <c r="D17" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E17" s="4">
+        <v>18</v>
+      </c>
+      <c r="F17" s="4">
+        <f>E17-G17</f>
+        <v>5</v>
+      </c>
+      <c r="G17" s="4">
+        <v>13</v>
+      </c>
+      <c r="H17" s="4"/>
+      <c r="I17" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="J17" s="4"/>
+    </row>
+    <row r="18" spans="2:10">
+      <c r="B18" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="C18" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="D18" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E18" s="4">
+        <f>SUM(E19:E23)</f>
+        <v>21</v>
+      </c>
+      <c r="F18" s="4">
+        <f t="shared" ref="F18:G18" si="6">SUM(F19:F23)</f>
+        <v>18</v>
+      </c>
+      <c r="G18" s="4">
+        <f t="shared" si="6"/>
+        <v>3</v>
+      </c>
+      <c r="H18" s="4">
+        <v>5</v>
+      </c>
+      <c r="I18" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="J18" s="5" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="19" spans="2:10">
+      <c r="B19" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="C19" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="D19" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E19" s="4">
+        <v>2</v>
+      </c>
+      <c r="F19" s="4">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="G19" s="4">
+        <v>2</v>
+      </c>
+      <c r="H19" s="4"/>
+      <c r="I19" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="J19" s="4"/>
+    </row>
+    <row r="20" spans="2:10">
+      <c r="B20" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="C20" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="D20" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E20" s="4">
+        <v>6</v>
+      </c>
+      <c r="F20" s="4">
         <f t="shared" si="1"/>
         <v>3</v>
       </c>
-      <c r="G16" s="4">
-        <v>0</v>
-      </c>
-      <c r="H16" s="4"/>
-      <c r="I16" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="J16" s="4"/>
-    </row>
-    <row r="17" spans="2:10">
-      <c r="B17" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="C17" s="7" t="s">
-        <v>37</v>
-      </c>
-      <c r="D17" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="E17" s="4">
-        <f>SUM(E18:E22)</f>
-        <v>21</v>
-      </c>
-      <c r="F17" s="4">
-        <f t="shared" ref="F17:G17" si="4">SUM(F18:F22)</f>
-        <v>18</v>
-      </c>
-      <c r="G17" s="4">
-        <f t="shared" si="4"/>
+      <c r="G20" s="4">
         <v>3</v>
       </c>
-      <c r="H17" s="4">
+      <c r="H20" s="4"/>
+      <c r="I20" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="J20" s="4"/>
+    </row>
+    <row r="21" spans="2:10">
+      <c r="B21" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="C21" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="D21" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E21" s="4">
+        <v>6</v>
+      </c>
+      <c r="F21" s="4">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="G21" s="4">
         <v>5</v>
       </c>
-      <c r="I17" s="4" t="s">
+      <c r="H21" s="4"/>
+      <c r="I21" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="J21" s="4"/>
+    </row>
+    <row r="22" spans="2:10">
+      <c r="B22" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="C22" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="D22" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E22" s="4">
+        <v>1</v>
+      </c>
+      <c r="F22" s="4">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="G22" s="4">
+        <v>1</v>
+      </c>
+      <c r="H22" s="4"/>
+      <c r="I22" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="J17" s="5" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="18" spans="2:10">
-      <c r="B18" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="C18" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="D18" s="4" t="s">
+      <c r="J22" s="4"/>
+    </row>
+    <row r="23" spans="2:10">
+      <c r="B23" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="C23" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="D23" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="E18" s="4">
-        <v>2</v>
-      </c>
-      <c r="F18" s="4">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="G18" s="4">
-        <v>2</v>
-      </c>
-      <c r="H18" s="4"/>
-      <c r="I18" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="J18" s="4"/>
-    </row>
-    <row r="19" spans="2:10">
-      <c r="B19" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="C19" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="D19" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="E19" s="4">
+      <c r="E23" s="4">
         <v>6</v>
       </c>
-      <c r="F19" s="4">
+      <c r="F23" s="4">
         <f t="shared" si="1"/>
         <v>6</v>
       </c>
-      <c r="G19" s="4">
-        <v>0</v>
-      </c>
-      <c r="H19" s="4"/>
-      <c r="I19" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="J19" s="4"/>
-    </row>
-    <row r="20" spans="2:10">
-      <c r="B20" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="C20" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="D20" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="E20" s="4">
-        <v>6</v>
-      </c>
-      <c r="F20" s="4">
-        <f t="shared" si="1"/>
-        <v>6</v>
-      </c>
-      <c r="G20" s="4">
-        <v>0</v>
-      </c>
-      <c r="H20" s="4"/>
-      <c r="I20" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="J20" s="4"/>
-    </row>
-    <row r="21" spans="2:10">
-      <c r="B21" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="C21" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="D21" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="E21" s="4">
-        <v>1</v>
-      </c>
-      <c r="F21" s="4">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="G21" s="4">
-        <v>1</v>
-      </c>
-      <c r="H21" s="4"/>
-      <c r="I21" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="J21" s="4"/>
-    </row>
-    <row r="22" spans="2:10">
-      <c r="B22" s="3" t="s">
+      <c r="G23" s="4">
+        <v>0</v>
+      </c>
+      <c r="H23" s="4"/>
+      <c r="I23" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="C22" s="4" t="s">
-        <v>92</v>
-      </c>
-      <c r="D22" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="E22" s="4">
-        <v>6</v>
-      </c>
-      <c r="F22" s="4">
-        <f t="shared" si="1"/>
-        <v>6</v>
-      </c>
-      <c r="G22" s="4">
-        <v>0</v>
-      </c>
-      <c r="H22" s="4"/>
-      <c r="I22" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="J22" s="4"/>
-    </row>
-    <row r="23" spans="2:10">
-      <c r="B23" s="6" t="s">
+      <c r="J23" s="4"/>
+    </row>
+    <row r="24" spans="2:10">
+      <c r="B24" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="C24" s="7" t="s">
         <v>50</v>
       </c>
-      <c r="C23" s="7" t="s">
-        <v>51</v>
-      </c>
-      <c r="D23" s="4" t="s">
+      <c r="D24" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="E23" s="4">
-        <f>SUM(E24:E26)</f>
+      <c r="E24" s="4">
+        <f>SUM(E25:E27)</f>
         <v>10</v>
-      </c>
-      <c r="F23" s="4">
-        <f t="shared" ref="F23:G23" si="5">SUM(F24:F26)</f>
-        <v>10</v>
-      </c>
-      <c r="G23" s="4">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="H23" s="4">
-        <v>5</v>
-      </c>
-      <c r="I23" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="J23" s="4" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="24" spans="2:10">
-      <c r="B24" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="C24" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="D24" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="E24" s="4">
-        <v>1</v>
       </c>
       <c r="F24" s="4">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="G24" s="4">
-        <v>0</v>
-      </c>
-      <c r="H24" s="4"/>
+        <f t="shared" ref="G24" si="7">SUM(G25:G27)</f>
+        <v>6</v>
+      </c>
+      <c r="H24" s="4">
+        <v>5</v>
+      </c>
       <c r="I24" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="J24" s="4"/>
+      <c r="J24" s="4" t="s">
+        <v>118</v>
+      </c>
     </row>
     <row r="25" spans="2:10">
       <c r="B25" s="3" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="C25" s="4" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="D25" s="4" t="s">
         <v>11</v>
       </c>
       <c r="E25" s="4">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="F25" s="4">
         <f t="shared" si="1"/>
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="G25" s="4">
         <v>0</v>
@@ -1785,23 +1835,23 @@
     </row>
     <row r="26" spans="2:10">
       <c r="B26" s="3" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="C26" s="4" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="D26" s="4" t="s">
         <v>11</v>
       </c>
       <c r="E26" s="4">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="F26" s="4">
         <f t="shared" si="1"/>
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="G26" s="4">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="H26" s="4"/>
       <c r="I26" s="4" t="s">
@@ -1810,237 +1860,304 @@
       <c r="J26" s="4"/>
     </row>
     <row r="27" spans="2:10">
-      <c r="B27" s="6" t="s">
-        <v>60</v>
-      </c>
-      <c r="C27" s="7" t="s">
-        <v>61</v>
+      <c r="B27" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="C27" s="4" t="s">
+        <v>57</v>
       </c>
       <c r="D27" s="4" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="E27" s="4">
-        <f>SUM(E28:E31)</f>
-        <v>16</v>
+        <v>3</v>
       </c>
       <c r="F27" s="4">
-        <f t="shared" ref="F27:G27" si="6">SUM(F28:F31)</f>
-        <v>16</v>
+        <f t="shared" si="1"/>
+        <v>3</v>
       </c>
       <c r="G27" s="4">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="H27" s="4">
-        <v>7</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="H27" s="4"/>
       <c r="I27" s="4" t="s">
-        <v>64</v>
-      </c>
-      <c r="J27" s="4" t="s">
-        <v>73</v>
-      </c>
+        <v>18</v>
+      </c>
+      <c r="J27" s="4"/>
     </row>
     <row r="28" spans="2:10">
       <c r="B28" s="3" t="s">
-        <v>66</v>
+        <v>116</v>
       </c>
       <c r="C28" s="4" t="s">
-        <v>28</v>
+        <v>117</v>
       </c>
       <c r="D28" s="4" t="s">
         <v>11</v>
       </c>
       <c r="E28" s="4">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="F28" s="4">
         <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
+      <c r="G28" s="4">
         <v>3</v>
-      </c>
-      <c r="G28" s="4">
-        <v>0</v>
       </c>
       <c r="H28" s="4"/>
       <c r="I28" s="4" t="s">
-        <v>64</v>
+        <v>30</v>
       </c>
       <c r="J28" s="4"/>
     </row>
     <row r="29" spans="2:10">
-      <c r="B29" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="C29" s="4" t="s">
-        <v>62</v>
+      <c r="B29" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="C29" s="7" t="s">
+        <v>60</v>
       </c>
       <c r="D29" s="4" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="E29" s="4">
-        <v>1</v>
+        <f>SUM(E30:E33)</f>
+        <v>10</v>
       </c>
       <c r="F29" s="4">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G29" s="4">
-        <v>0</v>
-      </c>
-      <c r="H29" s="4"/>
+        <f t="shared" ref="G29" si="8">SUM(G30:G33)</f>
+        <v>10</v>
+      </c>
+      <c r="H29" s="4">
+        <v>7</v>
+      </c>
       <c r="I29" s="4" t="s">
-        <v>64</v>
-      </c>
-      <c r="J29" s="4"/>
+        <v>63</v>
+      </c>
+      <c r="J29" s="4" t="s">
+        <v>72</v>
+      </c>
     </row>
     <row r="30" spans="2:10">
       <c r="B30" s="3" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="C30" s="4" t="s">
-        <v>63</v>
+        <v>28</v>
       </c>
       <c r="D30" s="4" t="s">
         <v>11</v>
       </c>
       <c r="E30" s="4">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="F30" s="4">
         <f t="shared" si="1"/>
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="G30" s="4">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="H30" s="4"/>
       <c r="I30" s="4" t="s">
-        <v>64</v>
+        <v>119</v>
       </c>
       <c r="J30" s="4"/>
     </row>
     <row r="31" spans="2:10">
       <c r="B31" s="3" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="C31" s="4" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="D31" s="4" t="s">
         <v>11</v>
       </c>
       <c r="E31" s="4">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="F31" s="4">
         <f t="shared" si="1"/>
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="G31" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H31" s="4"/>
       <c r="I31" s="4" t="s">
-        <v>64</v>
+        <v>30</v>
       </c>
       <c r="J31" s="4"/>
     </row>
     <row r="32" spans="2:10">
-      <c r="B32" s="6" t="s">
+      <c r="B32" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="C32" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="D32" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E32" s="4">
+        <v>6</v>
+      </c>
+      <c r="F32" s="4">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="G32" s="4">
+        <v>6</v>
+      </c>
+      <c r="H32" s="4"/>
+      <c r="I32" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="J32" s="4"/>
+    </row>
+    <row r="33" spans="2:10">
+      <c r="B33" s="3"/>
+      <c r="C33" s="4"/>
+      <c r="D33" s="4"/>
+      <c r="E33" s="4"/>
+      <c r="F33" s="4"/>
+      <c r="G33" s="4"/>
+      <c r="H33" s="4"/>
+      <c r="I33" s="4"/>
+      <c r="J33" s="4"/>
+    </row>
+    <row r="34" spans="2:10">
+      <c r="B34" s="6" t="s">
+        <v>108</v>
+      </c>
+      <c r="C34" s="7" t="s">
         <v>109</v>
       </c>
-      <c r="C32" s="7" t="s">
+      <c r="D34" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E34" s="4">
+        <f>SUM(E35:E38)</f>
+        <v>25</v>
+      </c>
+      <c r="F34" s="4">
+        <f t="shared" si="1"/>
+        <v>17</v>
+      </c>
+      <c r="G34" s="4">
+        <f t="shared" ref="G34" si="9">SUM(G35:G38)</f>
+        <v>8</v>
+      </c>
+      <c r="H34" s="4">
+        <v>6</v>
+      </c>
+      <c r="I34" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="J34" s="4" t="s">
         <v>110</v>
       </c>
-      <c r="D32" s="4" t="s">
+    </row>
+    <row r="35" spans="2:10">
+      <c r="B35" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="C35" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="D35" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E35" s="25">
+        <v>1</v>
+      </c>
+      <c r="F35" s="4">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="G35" s="25" t="s">
+        <v>111</v>
+      </c>
+      <c r="H35" s="3"/>
+      <c r="I35" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="J35" s="3"/>
+    </row>
+    <row r="36" spans="2:10">
+      <c r="B36" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="C36" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="D36" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E36" s="25">
+        <v>16</v>
+      </c>
+      <c r="F36" s="25">
+        <f t="shared" si="1"/>
         <v>8</v>
       </c>
-      <c r="E32" s="4">
-        <f>SUM(E33:E36)</f>
-        <v>1</v>
-      </c>
-      <c r="F32" s="4">
-        <f t="shared" ref="F32:G32" si="7">SUM(F33:F36)</f>
-        <v>0</v>
-      </c>
-      <c r="G32" s="4">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="H32" s="4">
-        <v>6</v>
-      </c>
-      <c r="I32" s="4" t="s">
+      <c r="G36" s="25">
+        <v>8</v>
+      </c>
+      <c r="H36" s="3"/>
+      <c r="I36" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="J32" s="4" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="33" spans="2:10">
-      <c r="B33" s="3" t="s">
-        <v>111</v>
-      </c>
-      <c r="C33" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="D33" s="3" t="s">
+      <c r="J36" s="3"/>
+    </row>
+    <row r="37" spans="2:10">
+      <c r="B37" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="C37" s="3" t="s">
+        <v>121</v>
+      </c>
+      <c r="D37" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="E33" s="39">
-        <v>1</v>
-      </c>
-      <c r="F33" s="39">
-        <f t="shared" ref="F33:F36" si="8">E33-G33</f>
-        <v>0</v>
-      </c>
-      <c r="G33" s="39" t="s">
-        <v>112</v>
-      </c>
-      <c r="H33" s="3"/>
-      <c r="I33" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="J33" s="3"/>
-    </row>
-    <row r="34" spans="2:10">
-      <c r="B34" s="37"/>
-      <c r="C34" s="38"/>
-      <c r="D34" s="38"/>
-      <c r="E34" s="38"/>
-      <c r="F34" s="38"/>
-      <c r="G34" s="38"/>
-      <c r="H34" s="38"/>
-      <c r="I34" s="38"/>
-      <c r="J34" s="38"/>
-    </row>
-    <row r="35" spans="2:10">
-      <c r="B35" s="37"/>
-      <c r="C35" s="38"/>
-      <c r="D35" s="38"/>
-      <c r="E35" s="38"/>
-      <c r="F35" s="38"/>
-      <c r="G35" s="38"/>
-      <c r="H35" s="38"/>
-      <c r="I35" s="38"/>
-      <c r="J35" s="38"/>
-    </row>
-    <row r="36" spans="2:10">
-      <c r="B36" s="37"/>
-      <c r="C36" s="38"/>
-      <c r="D36" s="38"/>
-      <c r="E36" s="38"/>
-      <c r="F36" s="38"/>
-      <c r="G36" s="38"/>
-      <c r="H36" s="38"/>
-      <c r="I36" s="38"/>
-      <c r="J36" s="38"/>
+      <c r="E37" s="25">
+        <v>8</v>
+      </c>
+      <c r="F37" s="25">
+        <f t="shared" si="1"/>
+        <v>8</v>
+      </c>
+      <c r="G37" s="25">
+        <v>0</v>
+      </c>
+      <c r="H37" s="3"/>
+      <c r="I37" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="J37" s="3"/>
+    </row>
+    <row r="38" spans="2:10">
+      <c r="B38" s="23"/>
+      <c r="C38" s="24"/>
+      <c r="D38" s="24"/>
+      <c r="E38" s="24"/>
+      <c r="F38" s="24"/>
+      <c r="G38" s="24"/>
+      <c r="H38" s="24"/>
+      <c r="I38" s="24"/>
+      <c r="J38" s="24"/>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="B2:J2"/>
   </mergeCells>
-  <conditionalFormatting sqref="H23:H27 H9:H21 H1 H3:H7 H29:H32 H34:H1048576">
+  <conditionalFormatting sqref="H24:H29 H9:H16 H1 H3:H7 H31:H34 H18:H22 H38:H1048576">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="num" val="0"/>
@@ -2079,52 +2196,52 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:5" ht="30.6" customHeight="1" thickBot="1">
-      <c r="B2" s="30" t="s">
-        <v>83</v>
-      </c>
-      <c r="C2" s="30"/>
-      <c r="D2" s="30"/>
-      <c r="E2" s="30"/>
+      <c r="B2" s="34" t="s">
+        <v>82</v>
+      </c>
+      <c r="C2" s="34"/>
+      <c r="D2" s="34"/>
+      <c r="E2" s="34"/>
     </row>
     <row r="3" spans="2:5" ht="15" thickBot="1">
       <c r="B3" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="24" t="s">
+      <c r="C3" s="28" t="s">
         <v>9</v>
       </c>
-      <c r="D3" s="25"/>
-      <c r="E3" s="26"/>
+      <c r="D3" s="29"/>
+      <c r="E3" s="30"/>
     </row>
     <row r="4" spans="2:5" ht="15" thickBot="1">
       <c r="B4" s="18" t="s">
-        <v>76</v>
-      </c>
-      <c r="C4" s="24" t="s">
+        <v>75</v>
+      </c>
+      <c r="C4" s="28" t="s">
         <v>10</v>
       </c>
-      <c r="D4" s="25"/>
-      <c r="E4" s="26"/>
+      <c r="D4" s="29"/>
+      <c r="E4" s="30"/>
     </row>
     <row r="5" spans="2:5" ht="15" thickBot="1">
       <c r="B5" s="18" t="s">
-        <v>79</v>
-      </c>
-      <c r="C5" s="24" t="s">
-        <v>49</v>
-      </c>
-      <c r="D5" s="25"/>
-      <c r="E5" s="26"/>
+        <v>78</v>
+      </c>
+      <c r="C5" s="28" t="s">
+        <v>48</v>
+      </c>
+      <c r="D5" s="29"/>
+      <c r="E5" s="30"/>
     </row>
     <row r="6" spans="2:5" ht="32.4" customHeight="1" thickBot="1">
       <c r="B6" s="18" t="s">
-        <v>77</v>
-      </c>
-      <c r="C6" s="27" t="s">
-        <v>108</v>
-      </c>
-      <c r="D6" s="28"/>
-      <c r="E6" s="29"/>
+        <v>76</v>
+      </c>
+      <c r="C6" s="31" t="s">
+        <v>107</v>
+      </c>
+      <c r="D6" s="32"/>
+      <c r="E6" s="33"/>
     </row>
     <row r="7" spans="2:5" ht="15" thickBot="1">
       <c r="B7" s="19" t="s">
@@ -2134,10 +2251,10 @@
         <v>0</v>
       </c>
       <c r="D7" s="11" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E7" s="12" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="8" spans="2:5">
@@ -2148,7 +2265,7 @@
         <v>19</v>
       </c>
       <c r="E8" s="14" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="9" spans="2:5">
@@ -2156,21 +2273,21 @@
         <v>13</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E9" s="14" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="10" spans="2:5" ht="15" thickBot="1">
       <c r="C10" s="15" t="s">
+        <v>45</v>
+      </c>
+      <c r="D10" s="16" t="s">
         <v>46</v>
       </c>
-      <c r="D10" s="16" t="s">
-        <v>47</v>
-      </c>
       <c r="E10" s="17" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
   </sheetData>
@@ -2207,52 +2324,52 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:5" ht="30.6" customHeight="1" thickBot="1">
-      <c r="B2" s="30" t="s">
-        <v>83</v>
-      </c>
-      <c r="C2" s="30"/>
-      <c r="D2" s="30"/>
-      <c r="E2" s="30"/>
+      <c r="B2" s="34" t="s">
+        <v>82</v>
+      </c>
+      <c r="C2" s="34"/>
+      <c r="D2" s="34"/>
+      <c r="E2" s="34"/>
     </row>
     <row r="3" spans="2:5" ht="15" thickBot="1">
       <c r="B3" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="24" t="s">
+      <c r="C3" s="28" t="s">
         <v>14</v>
       </c>
-      <c r="D3" s="25"/>
-      <c r="E3" s="26"/>
+      <c r="D3" s="29"/>
+      <c r="E3" s="30"/>
     </row>
     <row r="4" spans="2:5" ht="15" thickBot="1">
       <c r="B4" s="18" t="s">
-        <v>76</v>
-      </c>
-      <c r="C4" s="24" t="s">
+        <v>75</v>
+      </c>
+      <c r="C4" s="28" t="s">
         <v>15</v>
       </c>
-      <c r="D4" s="25"/>
-      <c r="E4" s="26"/>
+      <c r="D4" s="29"/>
+      <c r="E4" s="30"/>
     </row>
     <row r="5" spans="2:5" ht="15" thickBot="1">
       <c r="B5" s="18" t="s">
-        <v>79</v>
-      </c>
-      <c r="C5" s="24" t="s">
+        <v>78</v>
+      </c>
+      <c r="C5" s="28" t="s">
         <v>17</v>
       </c>
-      <c r="D5" s="25"/>
-      <c r="E5" s="26"/>
+      <c r="D5" s="29"/>
+      <c r="E5" s="30"/>
     </row>
     <row r="6" spans="2:5" ht="15" customHeight="1" thickBot="1">
       <c r="B6" s="18" t="s">
-        <v>77</v>
-      </c>
-      <c r="C6" s="31" t="s">
-        <v>84</v>
-      </c>
-      <c r="D6" s="32"/>
-      <c r="E6" s="33"/>
+        <v>76</v>
+      </c>
+      <c r="C6" s="35" t="s">
+        <v>83</v>
+      </c>
+      <c r="D6" s="36"/>
+      <c r="E6" s="37"/>
     </row>
     <row r="7" spans="2:5" ht="15" thickBot="1">
       <c r="B7" s="19" t="s">
@@ -2262,10 +2379,10 @@
         <v>0</v>
       </c>
       <c r="D7" s="11" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E7" s="12" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="8" spans="2:5" ht="43.8" thickBot="1">
@@ -2276,7 +2393,7 @@
         <v>20</v>
       </c>
       <c r="E8" s="20" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
   </sheetData>
@@ -2313,52 +2430,52 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:5" ht="30.6" customHeight="1" thickBot="1">
-      <c r="B2" s="30" t="s">
-        <v>83</v>
-      </c>
-      <c r="C2" s="30"/>
-      <c r="D2" s="30"/>
-      <c r="E2" s="30"/>
+      <c r="B2" s="34" t="s">
+        <v>82</v>
+      </c>
+      <c r="C2" s="34"/>
+      <c r="D2" s="34"/>
+      <c r="E2" s="34"/>
     </row>
     <row r="3" spans="2:5" ht="15" thickBot="1">
       <c r="B3" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="24" t="s">
+      <c r="C3" s="28" t="s">
         <v>21</v>
       </c>
-      <c r="D3" s="25"/>
-      <c r="E3" s="26"/>
+      <c r="D3" s="29"/>
+      <c r="E3" s="30"/>
     </row>
     <row r="4" spans="2:5" ht="15" thickBot="1">
       <c r="B4" s="18" t="s">
-        <v>76</v>
-      </c>
-      <c r="C4" s="24" t="s">
-        <v>36</v>
-      </c>
-      <c r="D4" s="25"/>
-      <c r="E4" s="26"/>
+        <v>75</v>
+      </c>
+      <c r="C4" s="28" t="s">
+        <v>35</v>
+      </c>
+      <c r="D4" s="29"/>
+      <c r="E4" s="30"/>
     </row>
     <row r="5" spans="2:5" ht="15" thickBot="1">
       <c r="B5" s="18" t="s">
-        <v>79</v>
-      </c>
-      <c r="C5" s="24" t="s">
-        <v>91</v>
-      </c>
-      <c r="D5" s="25"/>
-      <c r="E5" s="26"/>
+        <v>78</v>
+      </c>
+      <c r="C5" s="28" t="s">
+        <v>90</v>
+      </c>
+      <c r="D5" s="29"/>
+      <c r="E5" s="30"/>
     </row>
     <row r="6" spans="2:5" ht="15" customHeight="1" thickBot="1">
       <c r="B6" s="18" t="s">
+        <v>76</v>
+      </c>
+      <c r="C6" s="38" t="s">
         <v>77</v>
       </c>
-      <c r="C6" s="34" t="s">
-        <v>78</v>
-      </c>
-      <c r="D6" s="35"/>
-      <c r="E6" s="36"/>
+      <c r="D6" s="39"/>
+      <c r="E6" s="40"/>
     </row>
     <row r="7" spans="2:5" ht="15" thickBot="1">
       <c r="B7" s="19" t="s">
@@ -2368,10 +2485,10 @@
         <v>0</v>
       </c>
       <c r="D7" s="11" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E7" s="12" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="8" spans="2:5">
@@ -2382,7 +2499,7 @@
         <v>28</v>
       </c>
       <c r="E8" s="14" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="9" spans="2:5" ht="28.8">
@@ -2393,7 +2510,7 @@
         <v>26</v>
       </c>
       <c r="E9" s="21" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="10" spans="2:5" ht="28.8">
@@ -2404,7 +2521,7 @@
         <v>27</v>
       </c>
       <c r="E10" s="21" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="11" spans="2:5" ht="28.8">
@@ -2415,7 +2532,7 @@
         <v>31</v>
       </c>
       <c r="E11" s="21" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="12" spans="2:5" ht="29.4" thickBot="1">
@@ -2426,7 +2543,7 @@
         <v>33</v>
       </c>
       <c r="E12" s="20" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
   </sheetData>
@@ -2463,52 +2580,52 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:5" ht="30.6" customHeight="1" thickBot="1">
-      <c r="B2" s="30" t="s">
-        <v>83</v>
-      </c>
-      <c r="C2" s="30"/>
-      <c r="D2" s="30"/>
-      <c r="E2" s="30"/>
+      <c r="B2" s="34" t="s">
+        <v>82</v>
+      </c>
+      <c r="C2" s="34"/>
+      <c r="D2" s="34"/>
+      <c r="E2" s="34"/>
     </row>
     <row r="3" spans="2:5" ht="15" thickBot="1">
       <c r="B3" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="24" t="s">
-        <v>35</v>
-      </c>
-      <c r="D3" s="25"/>
-      <c r="E3" s="26"/>
+      <c r="C3" s="28" t="s">
+        <v>34</v>
+      </c>
+      <c r="D3" s="29"/>
+      <c r="E3" s="30"/>
     </row>
     <row r="4" spans="2:5" ht="15" thickBot="1">
       <c r="B4" s="18" t="s">
-        <v>76</v>
-      </c>
-      <c r="C4" s="24" t="s">
-        <v>37</v>
-      </c>
-      <c r="D4" s="25"/>
-      <c r="E4" s="26"/>
+        <v>75</v>
+      </c>
+      <c r="C4" s="28" t="s">
+        <v>36</v>
+      </c>
+      <c r="D4" s="29"/>
+      <c r="E4" s="30"/>
     </row>
     <row r="5" spans="2:5" ht="15" thickBot="1">
       <c r="B5" s="18" t="s">
-        <v>79</v>
-      </c>
-      <c r="C5" s="24" t="s">
-        <v>49</v>
-      </c>
-      <c r="D5" s="25"/>
-      <c r="E5" s="26"/>
+        <v>78</v>
+      </c>
+      <c r="C5" s="28" t="s">
+        <v>48</v>
+      </c>
+      <c r="D5" s="29"/>
+      <c r="E5" s="30"/>
     </row>
     <row r="6" spans="2:5" ht="15" customHeight="1" thickBot="1">
       <c r="B6" s="18" t="s">
-        <v>77</v>
-      </c>
-      <c r="C6" s="31" t="s">
-        <v>93</v>
-      </c>
-      <c r="D6" s="32"/>
-      <c r="E6" s="33"/>
+        <v>76</v>
+      </c>
+      <c r="C6" s="35" t="s">
+        <v>92</v>
+      </c>
+      <c r="D6" s="36"/>
+      <c r="E6" s="37"/>
     </row>
     <row r="7" spans="2:5" ht="15" thickBot="1">
       <c r="B7" s="19" t="s">
@@ -2518,65 +2635,65 @@
         <v>0</v>
       </c>
       <c r="D7" s="11" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E7" s="12" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="8" spans="2:5">
       <c r="C8" s="13" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D8" s="4" t="s">
         <v>28</v>
       </c>
       <c r="E8" s="14" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="9" spans="2:5" ht="28.8">
       <c r="C9" s="13" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E9" s="21" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="10" spans="2:5" ht="43.2">
       <c r="C10" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="D10" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="D10" s="4" t="s">
-        <v>43</v>
-      </c>
       <c r="E10" s="21" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="11" spans="2:5">
       <c r="C11" s="13" t="s">
+        <v>43</v>
+      </c>
+      <c r="D11" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="D11" s="4" t="s">
-        <v>45</v>
-      </c>
       <c r="E11" s="14" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="12" spans="2:5" ht="29.4" thickBot="1">
       <c r="C12" s="15" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D12" s="16" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E12" s="20" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
   </sheetData>
@@ -2613,52 +2730,52 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:5" ht="30.6" customHeight="1" thickBot="1">
-      <c r="B2" s="30" t="s">
-        <v>83</v>
-      </c>
-      <c r="C2" s="30"/>
-      <c r="D2" s="30"/>
-      <c r="E2" s="30"/>
+      <c r="B2" s="34" t="s">
+        <v>82</v>
+      </c>
+      <c r="C2" s="34"/>
+      <c r="D2" s="34"/>
+      <c r="E2" s="34"/>
     </row>
     <row r="3" spans="2:5" ht="15" thickBot="1">
       <c r="B3" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="24" t="s">
-        <v>50</v>
-      </c>
-      <c r="D3" s="25"/>
-      <c r="E3" s="26"/>
+      <c r="C3" s="28" t="s">
+        <v>49</v>
+      </c>
+      <c r="D3" s="29"/>
+      <c r="E3" s="30"/>
     </row>
     <row r="4" spans="2:5" ht="15" thickBot="1">
       <c r="B4" s="18" t="s">
-        <v>76</v>
-      </c>
-      <c r="C4" s="24" t="s">
-        <v>51</v>
-      </c>
-      <c r="D4" s="25"/>
-      <c r="E4" s="26"/>
+        <v>75</v>
+      </c>
+      <c r="C4" s="28" t="s">
+        <v>50</v>
+      </c>
+      <c r="D4" s="29"/>
+      <c r="E4" s="30"/>
     </row>
     <row r="5" spans="2:5" ht="15" thickBot="1">
       <c r="B5" s="18" t="s">
-        <v>79</v>
-      </c>
-      <c r="C5" s="24" t="s">
-        <v>72</v>
-      </c>
-      <c r="D5" s="25"/>
-      <c r="E5" s="26"/>
+        <v>78</v>
+      </c>
+      <c r="C5" s="28" t="s">
+        <v>71</v>
+      </c>
+      <c r="D5" s="29"/>
+      <c r="E5" s="30"/>
     </row>
     <row r="6" spans="2:5" ht="15" customHeight="1" thickBot="1">
       <c r="B6" s="18" t="s">
-        <v>77</v>
-      </c>
-      <c r="C6" s="31" t="s">
-        <v>99</v>
-      </c>
-      <c r="D6" s="32"/>
-      <c r="E6" s="33"/>
+        <v>76</v>
+      </c>
+      <c r="C6" s="35" t="s">
+        <v>98</v>
+      </c>
+      <c r="D6" s="36"/>
+      <c r="E6" s="37"/>
     </row>
     <row r="7" spans="2:5" ht="15" thickBot="1">
       <c r="B7" s="19" t="s">
@@ -2668,43 +2785,43 @@
         <v>0</v>
       </c>
       <c r="D7" s="11" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E7" s="12" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="8" spans="2:5">
       <c r="C8" s="13" t="s">
+        <v>53</v>
+      </c>
+      <c r="D8" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="D8" s="4" t="s">
-        <v>55</v>
-      </c>
       <c r="E8" s="14" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="9" spans="2:5" ht="43.2">
       <c r="C9" s="13" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E9" s="21" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="10" spans="2:5" ht="43.8" thickBot="1">
       <c r="C10" s="15" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D10" s="16" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E10" s="20" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
   </sheetData>
@@ -2741,52 +2858,52 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:5" ht="30.6" customHeight="1" thickBot="1">
-      <c r="B2" s="30" t="s">
-        <v>83</v>
-      </c>
-      <c r="C2" s="30"/>
-      <c r="D2" s="30"/>
-      <c r="E2" s="30"/>
+      <c r="B2" s="34" t="s">
+        <v>82</v>
+      </c>
+      <c r="C2" s="34"/>
+      <c r="D2" s="34"/>
+      <c r="E2" s="34"/>
     </row>
     <row r="3" spans="2:5" ht="15" thickBot="1">
       <c r="B3" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="24" t="s">
-        <v>60</v>
-      </c>
-      <c r="D3" s="25"/>
-      <c r="E3" s="26"/>
+      <c r="C3" s="28" t="s">
+        <v>59</v>
+      </c>
+      <c r="D3" s="29"/>
+      <c r="E3" s="30"/>
     </row>
     <row r="4" spans="2:5" ht="15" thickBot="1">
       <c r="B4" s="18" t="s">
-        <v>76</v>
-      </c>
-      <c r="C4" s="24" t="s">
-        <v>61</v>
-      </c>
-      <c r="D4" s="25"/>
-      <c r="E4" s="26"/>
+        <v>75</v>
+      </c>
+      <c r="C4" s="28" t="s">
+        <v>60</v>
+      </c>
+      <c r="D4" s="29"/>
+      <c r="E4" s="30"/>
     </row>
     <row r="5" spans="2:5" ht="15" thickBot="1">
       <c r="B5" s="18" t="s">
-        <v>79</v>
-      </c>
-      <c r="C5" s="24" t="s">
-        <v>73</v>
-      </c>
-      <c r="D5" s="25"/>
-      <c r="E5" s="26"/>
+        <v>78</v>
+      </c>
+      <c r="C5" s="28" t="s">
+        <v>72</v>
+      </c>
+      <c r="D5" s="29"/>
+      <c r="E5" s="30"/>
     </row>
     <row r="6" spans="2:5" ht="15" customHeight="1" thickBot="1">
       <c r="B6" s="18" t="s">
-        <v>77</v>
-      </c>
-      <c r="C6" s="31" t="s">
-        <v>103</v>
-      </c>
-      <c r="D6" s="32"/>
-      <c r="E6" s="33"/>
+        <v>76</v>
+      </c>
+      <c r="C6" s="35" t="s">
+        <v>102</v>
+      </c>
+      <c r="D6" s="36"/>
+      <c r="E6" s="37"/>
     </row>
     <row r="7" spans="2:5" ht="15" thickBot="1">
       <c r="B7" s="19" t="s">
@@ -2796,54 +2913,54 @@
         <v>0</v>
       </c>
       <c r="D7" s="11" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E7" s="12" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="8" spans="2:5">
       <c r="C8" s="13" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D8" s="4" t="s">
         <v>28</v>
       </c>
       <c r="E8" s="14" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="9" spans="2:5" ht="28.8">
       <c r="C9" s="13" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E9" s="21" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="10" spans="2:5" ht="28.8">
       <c r="C10" s="13" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E10" s="21" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="11" spans="2:5" ht="29.4" thickBot="1">
       <c r="C11" s="15" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D11" s="16" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E11" s="20" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
   </sheetData>
@@ -2865,7 +2982,7 @@
   </sheetPr>
   <dimension ref="B2:E12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
@@ -2880,52 +2997,52 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:5" ht="30.6" customHeight="1" thickBot="1">
-      <c r="B2" s="30" t="s">
-        <v>83</v>
-      </c>
-      <c r="C2" s="30"/>
-      <c r="D2" s="30"/>
-      <c r="E2" s="30"/>
+      <c r="B2" s="34" t="s">
+        <v>82</v>
+      </c>
+      <c r="C2" s="34"/>
+      <c r="D2" s="34"/>
+      <c r="E2" s="34"/>
     </row>
     <row r="3" spans="2:5" ht="15" thickBot="1">
       <c r="B3" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="24" t="s">
-        <v>109</v>
-      </c>
-      <c r="D3" s="25"/>
-      <c r="E3" s="26"/>
+      <c r="C3" s="28" t="s">
+        <v>108</v>
+      </c>
+      <c r="D3" s="29"/>
+      <c r="E3" s="30"/>
     </row>
     <row r="4" spans="2:5" ht="15" thickBot="1">
       <c r="B4" s="18" t="s">
-        <v>76</v>
-      </c>
-      <c r="C4" s="24" t="s">
-        <v>110</v>
-      </c>
-      <c r="D4" s="25"/>
-      <c r="E4" s="26"/>
+        <v>75</v>
+      </c>
+      <c r="C4" s="28" t="s">
+        <v>109</v>
+      </c>
+      <c r="D4" s="29"/>
+      <c r="E4" s="30"/>
     </row>
     <row r="5" spans="2:5" ht="15" thickBot="1">
       <c r="B5" s="18" t="s">
-        <v>79</v>
-      </c>
-      <c r="C5" s="24" t="s">
-        <v>111</v>
-      </c>
-      <c r="D5" s="25"/>
-      <c r="E5" s="26"/>
+        <v>78</v>
+      </c>
+      <c r="C5" s="28" t="s">
+        <v>110</v>
+      </c>
+      <c r="D5" s="29"/>
+      <c r="E5" s="30"/>
     </row>
     <row r="6" spans="2:5" ht="15" customHeight="1" thickBot="1">
       <c r="B6" s="18" t="s">
-        <v>77</v>
-      </c>
-      <c r="C6" s="34" t="s">
-        <v>113</v>
-      </c>
-      <c r="D6" s="35"/>
-      <c r="E6" s="36"/>
+        <v>76</v>
+      </c>
+      <c r="C6" s="38" t="s">
+        <v>112</v>
+      </c>
+      <c r="D6" s="39"/>
+      <c r="E6" s="40"/>
     </row>
     <row r="7" spans="2:5" ht="15" thickBot="1">
       <c r="B7" s="19" t="s">
@@ -2935,42 +3052,42 @@
         <v>0</v>
       </c>
       <c r="D7" s="11" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E7" s="12" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="8" spans="2:5" ht="15" thickBot="1">
       <c r="C8" s="15" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D8" s="16" t="s">
         <v>28</v>
       </c>
       <c r="E8" s="17" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="9" spans="2:5">
-      <c r="C9" s="37"/>
-      <c r="D9" s="38"/>
-      <c r="E9" s="40"/>
+      <c r="C9" s="23"/>
+      <c r="D9" s="24"/>
+      <c r="E9" s="26"/>
     </row>
     <row r="10" spans="2:5">
-      <c r="C10" s="37"/>
-      <c r="D10" s="38"/>
-      <c r="E10" s="40"/>
+      <c r="C10" s="23"/>
+      <c r="D10" s="24"/>
+      <c r="E10" s="26"/>
     </row>
     <row r="11" spans="2:5">
-      <c r="C11" s="37"/>
-      <c r="D11" s="38"/>
-      <c r="E11" s="40"/>
+      <c r="C11" s="23"/>
+      <c r="D11" s="24"/>
+      <c r="E11" s="26"/>
     </row>
     <row r="12" spans="2:5">
-      <c r="C12" s="38"/>
-      <c r="D12" s="38"/>
-      <c r="E12" s="38"/>
+      <c r="C12" s="24"/>
+      <c r="D12" s="24"/>
+      <c r="E12" s="24"/>
     </row>
   </sheetData>
   <mergeCells count="5">

</xml_diff>